<commit_message>
Update blackbox testcase v2.0
</commit_message>
<xml_diff>
--- a/Docs/SE07_BlackBoxTestCase_v2.0.xlsx
+++ b/Docs/SE07_BlackBoxTestCase_v2.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4155" tabRatio="840" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4155" tabRatio="840"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -1012,7 +1012,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3219" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3222" uniqueCount="1373">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -5742,6 +5742,15 @@
     <t>- Tại màn hình quản lý kỳ thi - Cập nhật
 1. Nhập vào toàn bộ những thông tin cần thiết với độ dài lớn hơn lớn nhất
 2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>26/11/2016</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Update version 2.0</t>
   </si>
 </sst>
 </file>
@@ -5752,7 +5761,7 @@
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -5899,6 +5908,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -6941,7 +6957,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="628">
+  <cellXfs count="629">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -8561,6 +8577,20 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="62" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8646,20 +8676,9 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="62" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9060,8 +9079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9079,13 +9098,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="593" t="s">
+      <c r="C2" s="599" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="593"/>
-      <c r="E2" s="593"/>
-      <c r="F2" s="593"/>
-      <c r="G2" s="593"/>
+      <c r="D2" s="599"/>
+      <c r="E2" s="599"/>
+      <c r="F2" s="599"/>
+      <c r="G2" s="599"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -9096,11 +9115,11 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="594" t="s">
+      <c r="C4" s="600" t="s">
         <v>1316</v>
       </c>
-      <c r="D4" s="594"/>
-      <c r="E4" s="594"/>
+      <c r="D4" s="600"/>
+      <c r="E4" s="600"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
@@ -9112,26 +9131,26 @@
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="594" t="s">
+      <c r="C5" s="600" t="s">
         <v>1318</v>
       </c>
-      <c r="D5" s="594"/>
-      <c r="E5" s="594"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="600"/>
       <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="595" t="s">
+      <c r="B6" s="601" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="596" t="str">
+      <c r="C6" s="602" t="str">
         <f>C5&amp;"_"&amp;"TestReport"&amp;"_"&amp;"v1.0"</f>
         <v>HTTTNTT_TestReport_v1.0</v>
       </c>
-      <c r="D6" s="596"/>
-      <c r="E6" s="596"/>
+      <c r="D6" s="602"/>
+      <c r="E6" s="602"/>
       <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
@@ -9140,10 +9159,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="595"/>
-      <c r="C7" s="596"/>
-      <c r="D7" s="596"/>
-      <c r="E7" s="596"/>
+      <c r="B7" s="601"/>
+      <c r="C7" s="602"/>
+      <c r="D7" s="602"/>
+      <c r="E7" s="602"/>
       <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
@@ -9206,11 +9225,17 @@
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:7" s="25" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B13" s="30"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="628" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>1371</v>
+      </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
+      <c r="F13" s="27" t="s">
+        <v>1372</v>
+      </c>
       <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" s="25" customFormat="1" ht="19.5" customHeight="1">
@@ -9307,13 +9332,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -9325,13 +9350,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -9343,11 +9368,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -9366,10 +9391,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -9393,10 +9418,10 @@
         <f>COUNTIF(F$10:F$1012,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>18</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -9912,13 +9937,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>319</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -9930,13 +9955,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -9948,11 +9973,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -9971,10 +9996,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -9998,10 +10023,10 @@
         <f>COUNTIF(F$10:F$1005,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>6</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -10077,10 +10102,10 @@
       <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="608" t="s">
+      <c r="A11" s="614" t="s">
         <v>324</v>
       </c>
-      <c r="B11" s="608" t="s">
+      <c r="B11" s="614" t="s">
         <v>98</v>
       </c>
       <c r="C11" s="135"/>
@@ -10096,8 +10121,8 @@
       <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="609"/>
-      <c r="B12" s="609"/>
+      <c r="A12" s="615"/>
+      <c r="B12" s="615"/>
       <c r="C12" s="135" t="s">
         <v>327</v>
       </c>
@@ -10111,8 +10136,8 @@
       <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="609"/>
-      <c r="B13" s="609"/>
+      <c r="A13" s="615"/>
+      <c r="B13" s="615"/>
       <c r="C13" s="135" t="s">
         <v>320</v>
       </c>
@@ -10126,8 +10151,8 @@
       <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="609"/>
-      <c r="B14" s="609"/>
+      <c r="A14" s="615"/>
+      <c r="B14" s="615"/>
       <c r="C14" s="136" t="s">
         <v>328</v>
       </c>
@@ -10141,8 +10166,8 @@
       <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:10" ht="25.5">
-      <c r="A15" s="609"/>
-      <c r="B15" s="609"/>
+      <c r="A15" s="615"/>
+      <c r="B15" s="615"/>
       <c r="C15" s="136" t="s">
         <v>329</v>
       </c>
@@ -10156,8 +10181,8 @@
       <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:10" ht="25.5">
-      <c r="A16" s="609"/>
-      <c r="B16" s="609"/>
+      <c r="A16" s="615"/>
+      <c r="B16" s="615"/>
       <c r="C16" s="136" t="s">
         <v>330</v>
       </c>
@@ -10171,8 +10196,8 @@
       <c r="I16" s="77"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="610"/>
-      <c r="B17" s="610"/>
+      <c r="A17" s="616"/>
+      <c r="B17" s="616"/>
       <c r="C17" s="136" t="s">
         <v>104</v>
       </c>
@@ -10347,13 +10372,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1303</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -10365,13 +10390,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -10383,11 +10408,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -10406,10 +10431,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -10433,10 +10458,10 @@
         <f>COUNTIF(F$10:F$1015,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>21</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -11023,13 +11048,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>409</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -11041,13 +11066,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -11059,11 +11084,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -11082,10 +11107,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -11109,10 +11134,10 @@
         <f>COUNTIF(F$10:F$1013,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>21</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -11674,13 +11699,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>455</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -11692,13 +11717,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -11710,11 +11735,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -11733,10 +11758,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -11760,10 +11785,10 @@
         <f>COUNTIF(F$10:F$1005,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>6</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -11839,10 +11864,10 @@
       <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="608" t="s">
+      <c r="A11" s="614" t="s">
         <v>459</v>
       </c>
-      <c r="B11" s="608" t="s">
+      <c r="B11" s="614" t="s">
         <v>98</v>
       </c>
       <c r="C11" s="135"/>
@@ -11858,8 +11883,8 @@
       <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="609"/>
-      <c r="B12" s="609"/>
+      <c r="A12" s="615"/>
+      <c r="B12" s="615"/>
       <c r="C12" s="135" t="s">
         <v>462</v>
       </c>
@@ -11873,8 +11898,8 @@
       <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="609"/>
-      <c r="B13" s="609"/>
+      <c r="A13" s="615"/>
+      <c r="B13" s="615"/>
       <c r="C13" s="135" t="s">
         <v>328</v>
       </c>
@@ -11888,8 +11913,8 @@
       <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="609"/>
-      <c r="B14" s="609"/>
+      <c r="A14" s="615"/>
+      <c r="B14" s="615"/>
       <c r="C14" s="136" t="s">
         <v>329</v>
       </c>
@@ -11903,8 +11928,8 @@
       <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:10" ht="25.5">
-      <c r="A15" s="609"/>
-      <c r="B15" s="609"/>
+      <c r="A15" s="615"/>
+      <c r="B15" s="615"/>
       <c r="C15" s="136" t="s">
         <v>330</v>
       </c>
@@ -11918,8 +11943,8 @@
       <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:10" ht="25.5">
-      <c r="A16" s="609"/>
-      <c r="B16" s="609"/>
+      <c r="A16" s="615"/>
+      <c r="B16" s="615"/>
       <c r="C16" s="136" t="s">
         <v>463</v>
       </c>
@@ -11933,8 +11958,8 @@
       <c r="I16" s="77"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="610"/>
-      <c r="B17" s="610"/>
+      <c r="A17" s="616"/>
+      <c r="B17" s="616"/>
       <c r="C17" s="136" t="s">
         <v>104</v>
       </c>
@@ -12109,13 +12134,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>482</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -12127,13 +12152,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -12145,11 +12170,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -12168,10 +12193,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -12195,10 +12220,10 @@
         <f>COUNTIF(F$10:F$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>22</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -12782,13 +12807,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>538</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -12800,13 +12825,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -12818,11 +12843,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -12841,10 +12866,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -12868,10 +12893,10 @@
         <f>COUNTIF(F$10:F$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>22</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -13455,13 +13480,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>559</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -13473,13 +13498,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -13491,11 +13516,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -13514,10 +13539,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -13541,10 +13566,10 @@
         <f>COUNTIF(F$10:F$1005,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>6</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -13620,10 +13645,10 @@
       <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="608" t="s">
+      <c r="A11" s="614" t="s">
         <v>563</v>
       </c>
-      <c r="B11" s="608" t="s">
+      <c r="B11" s="614" t="s">
         <v>98</v>
       </c>
       <c r="C11" s="135"/>
@@ -13639,8 +13664,8 @@
       <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="609"/>
-      <c r="B12" s="609"/>
+      <c r="A12" s="615"/>
+      <c r="B12" s="615"/>
       <c r="C12" s="135" t="s">
         <v>566</v>
       </c>
@@ -13654,8 +13679,8 @@
       <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="609"/>
-      <c r="B13" s="609"/>
+      <c r="A13" s="615"/>
+      <c r="B13" s="615"/>
       <c r="C13" s="135" t="s">
         <v>463</v>
       </c>
@@ -13669,8 +13694,8 @@
       <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="609"/>
-      <c r="B14" s="609"/>
+      <c r="A14" s="615"/>
+      <c r="B14" s="615"/>
       <c r="C14" s="136" t="s">
         <v>567</v>
       </c>
@@ -13684,8 +13709,8 @@
       <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:10" ht="25.5">
-      <c r="A15" s="609"/>
-      <c r="B15" s="609"/>
+      <c r="A15" s="615"/>
+      <c r="B15" s="615"/>
       <c r="C15" s="136" t="s">
         <v>568</v>
       </c>
@@ -13699,8 +13724,8 @@
       <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:10" ht="25.5">
-      <c r="A16" s="609"/>
-      <c r="B16" s="609"/>
+      <c r="A16" s="615"/>
+      <c r="B16" s="615"/>
       <c r="C16" s="136" t="s">
         <v>569</v>
       </c>
@@ -13714,8 +13739,8 @@
       <c r="I16" s="77"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="610"/>
-      <c r="B17" s="610"/>
+      <c r="A17" s="616"/>
+      <c r="B17" s="616"/>
       <c r="C17" s="136" t="s">
         <v>104</v>
       </c>
@@ -13890,13 +13915,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>575</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -13908,13 +13933,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -13926,11 +13951,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -13949,10 +13974,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -13976,10 +14001,10 @@
         <f>COUNTIF(F$10:F$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>22</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -14563,13 +14588,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>632</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -14581,13 +14606,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -14599,11 +14624,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -14622,10 +14647,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -14649,10 +14674,10 @@
         <f>COUNTIF(F$10:F$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>22</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -15230,37 +15255,37 @@
       <c r="E2" s="39"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="599" t="s">
+      <c r="B3" s="605" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="599"/>
-      <c r="D3" s="600" t="s">
+      <c r="C3" s="605"/>
+      <c r="D3" s="606" t="s">
         <v>1316</v>
       </c>
-      <c r="E3" s="600"/>
-      <c r="F3" s="600"/>
+      <c r="E3" s="606"/>
+      <c r="F3" s="606"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="599" t="s">
+      <c r="B4" s="605" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="599"/>
-      <c r="D4" s="600" t="s">
+      <c r="C4" s="605"/>
+      <c r="D4" s="606" t="s">
         <v>1318</v>
       </c>
-      <c r="E4" s="600"/>
-      <c r="F4" s="600"/>
+      <c r="E4" s="606"/>
+      <c r="F4" s="606"/>
     </row>
     <row r="5" spans="2:6" s="40" customFormat="1" ht="84.75" customHeight="1">
-      <c r="B5" s="597" t="s">
+      <c r="B5" s="603" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="597"/>
-      <c r="D5" s="598" t="s">
+      <c r="C5" s="603"/>
+      <c r="D5" s="604" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="598"/>
-      <c r="F5" s="598"/>
+      <c r="E5" s="604"/>
+      <c r="F5" s="604"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="209"/>
@@ -15378,7 +15403,7 @@
       <c r="C15" s="166" t="s">
         <v>1352</v>
       </c>
-      <c r="D15" s="627" t="s">
+      <c r="D15" s="598" t="s">
         <v>1358</v>
       </c>
       <c r="E15" s="164"/>
@@ -15391,7 +15416,7 @@
       <c r="C16" s="166" t="s">
         <v>1355</v>
       </c>
-      <c r="D16" s="627" t="s">
+      <c r="D16" s="598" t="s">
         <v>1358</v>
       </c>
       <c r="E16" s="164"/>
@@ -15404,7 +15429,7 @@
       <c r="C17" s="162" t="s">
         <v>1357</v>
       </c>
-      <c r="D17" s="627" t="s">
+      <c r="D17" s="598" t="s">
         <v>1358</v>
       </c>
       <c r="E17" s="164"/>
@@ -16435,13 +16460,13 @@
       <c r="A2" s="507" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1146</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -16453,13 +16478,13 @@
       <c r="A3" s="508" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -16471,11 +16496,11 @@
       <c r="A4" s="507" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -16494,10 +16519,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -16522,11 +16547,11 @@
         <f>COUNTIF(F$10:F$1005,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1012)</f>
         <v>11</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -16583,10 +16608,10 @@
       <c r="I9" s="515"/>
     </row>
     <row r="10" spans="1:10" ht="25.5">
-      <c r="A10" s="611" t="s">
+      <c r="A10" s="617" t="s">
         <v>1148</v>
       </c>
-      <c r="B10" s="611" t="s">
+      <c r="B10" s="617" t="s">
         <v>98</v>
       </c>
       <c r="C10" s="453"/>
@@ -16602,8 +16627,8 @@
       <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="611"/>
-      <c r="B11" s="611"/>
+      <c r="A11" s="617"/>
+      <c r="B11" s="617"/>
       <c r="C11" s="453" t="s">
         <v>1150</v>
       </c>
@@ -16617,8 +16642,8 @@
       <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="611"/>
-      <c r="B12" s="611"/>
+      <c r="A12" s="617"/>
+      <c r="B12" s="617"/>
       <c r="C12" s="453" t="s">
         <v>1152</v>
       </c>
@@ -16632,8 +16657,8 @@
       <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="611"/>
-      <c r="B13" s="611"/>
+      <c r="A13" s="617"/>
+      <c r="B13" s="617"/>
       <c r="C13" s="453" t="s">
         <v>1154</v>
       </c>
@@ -16647,8 +16672,8 @@
       <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="611"/>
-      <c r="B14" s="611"/>
+      <c r="A14" s="617"/>
+      <c r="B14" s="617"/>
       <c r="C14" s="453" t="s">
         <v>1156</v>
       </c>
@@ -16662,8 +16687,8 @@
       <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="611"/>
-      <c r="B15" s="611"/>
+      <c r="A15" s="617"/>
+      <c r="B15" s="617"/>
       <c r="C15" s="453" t="s">
         <v>1158</v>
       </c>
@@ -16677,8 +16702,8 @@
       <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="611"/>
-      <c r="B16" s="611"/>
+      <c r="A16" s="617"/>
+      <c r="B16" s="617"/>
       <c r="D16" s="124"/>
       <c r="E16" s="125"/>
       <c r="F16" s="388"/>
@@ -16764,15 +16789,15 @@
     </row>
     <row r="21" spans="1:11" s="52" customFormat="1">
       <c r="A21" s="550"/>
-      <c r="B21" s="612" t="s">
+      <c r="B21" s="618" t="s">
         <v>1165</v>
       </c>
-      <c r="C21" s="613"/>
-      <c r="D21" s="613"/>
-      <c r="E21" s="613"/>
-      <c r="F21" s="613"/>
-      <c r="G21" s="613"/>
-      <c r="H21" s="614"/>
+      <c r="C21" s="619"/>
+      <c r="D21" s="619"/>
+      <c r="E21" s="619"/>
+      <c r="F21" s="619"/>
+      <c r="G21" s="619"/>
+      <c r="H21" s="620"/>
       <c r="I21" s="515"/>
     </row>
     <row r="22" spans="1:11" ht="63.75">
@@ -16961,13 +16986,13 @@
       <c r="A2" s="507" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1185</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -16979,13 +17004,13 @@
       <c r="A3" s="508" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -16997,11 +17022,11 @@
       <c r="A4" s="507" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -17020,10 +17045,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -17048,11 +17073,11 @@
         <f>COUNTIF(F$10:F$995,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1002)</f>
         <v>7</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -17167,15 +17192,15 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="550"/>
-      <c r="B13" s="612" t="s">
+      <c r="B13" s="618" t="s">
         <v>1192</v>
       </c>
-      <c r="C13" s="613"/>
-      <c r="D13" s="613"/>
-      <c r="E13" s="613"/>
-      <c r="F13" s="613"/>
-      <c r="G13" s="613"/>
-      <c r="H13" s="614"/>
+      <c r="C13" s="619"/>
+      <c r="D13" s="619"/>
+      <c r="E13" s="619"/>
+      <c r="F13" s="619"/>
+      <c r="G13" s="619"/>
+      <c r="H13" s="620"/>
       <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="38.25">
@@ -17351,13 +17376,13 @@
       <c r="A2" s="507" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1209</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -17369,13 +17394,13 @@
       <c r="A3" s="508" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -17387,11 +17412,11 @@
       <c r="A4" s="507" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -17410,10 +17435,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -17438,11 +17463,11 @@
         <f>COUNTIF(F$10:F$998,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1005)</f>
         <v>9</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -17576,15 +17601,15 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="550"/>
-      <c r="B14" s="612" t="s">
+      <c r="B14" s="618" t="s">
         <v>1273</v>
       </c>
-      <c r="C14" s="613"/>
-      <c r="D14" s="613"/>
-      <c r="E14" s="613"/>
-      <c r="F14" s="613"/>
-      <c r="G14" s="613"/>
-      <c r="H14" s="614"/>
+      <c r="C14" s="619"/>
+      <c r="D14" s="619"/>
+      <c r="E14" s="619"/>
+      <c r="F14" s="619"/>
+      <c r="G14" s="619"/>
+      <c r="H14" s="620"/>
       <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:10" ht="51">
@@ -17786,13 +17811,13 @@
       <c r="A2" s="507" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1234</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -17804,13 +17829,13 @@
       <c r="A3" s="508" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -17822,11 +17847,11 @@
       <c r="A4" s="507" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -17845,10 +17870,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -17873,11 +17898,11 @@
         <f>COUNTIF(F$10:F$991,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A998)</f>
         <v>3</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -17954,15 +17979,15 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="550"/>
-      <c r="B11" s="612" t="s">
+      <c r="B11" s="618" t="s">
         <v>1274</v>
       </c>
-      <c r="C11" s="613"/>
-      <c r="D11" s="613"/>
-      <c r="E11" s="613"/>
-      <c r="F11" s="613"/>
-      <c r="G11" s="613"/>
-      <c r="H11" s="614"/>
+      <c r="C11" s="619"/>
+      <c r="D11" s="619"/>
+      <c r="E11" s="619"/>
+      <c r="F11" s="619"/>
+      <c r="G11" s="619"/>
+      <c r="H11" s="620"/>
       <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:10" ht="38.25">
@@ -18098,35 +18123,35 @@
       <c r="A2" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="615" t="s">
+      <c r="B2" s="621" t="s">
         <v>698</v>
       </c>
-      <c r="C2" s="615"/>
-      <c r="D2" s="615"/>
-      <c r="E2" s="615"/>
-      <c r="F2" s="615"/>
+      <c r="C2" s="621"/>
+      <c r="D2" s="621"/>
+      <c r="E2" s="621"/>
+      <c r="F2" s="621"/>
     </row>
     <row r="3" spans="1:8" ht="38.25">
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
     </row>
     <row r="4" spans="1:8" ht="14.25">
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -18141,10 +18166,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -18163,11 +18188,11 @@
         <f>COUNTIF(F$10:F$1004,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1004)</f>
         <v>6</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -18226,10 +18251,10 @@
       <c r="H10" s="84"/>
     </row>
     <row r="11" spans="1:8" ht="38.25">
-      <c r="A11" s="608" t="s">
+      <c r="A11" s="614" t="s">
         <v>695</v>
       </c>
-      <c r="B11" s="608" t="s">
+      <c r="B11" s="614" t="s">
         <v>98</v>
       </c>
       <c r="C11" s="135"/>
@@ -18244,8 +18269,8 @@
       <c r="H11" s="84"/>
     </row>
     <row r="12" spans="1:8" ht="25.5">
-      <c r="A12" s="609"/>
-      <c r="B12" s="609"/>
+      <c r="A12" s="615"/>
+      <c r="B12" s="615"/>
       <c r="C12" s="135" t="s">
         <v>694</v>
       </c>
@@ -18258,8 +18283,8 @@
       <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="25.5">
-      <c r="A13" s="609"/>
-      <c r="B13" s="609"/>
+      <c r="A13" s="615"/>
+      <c r="B13" s="615"/>
       <c r="C13" s="135" t="s">
         <v>692</v>
       </c>
@@ -18272,8 +18297,8 @@
       <c r="H13" s="84"/>
     </row>
     <row r="14" spans="1:8" ht="25.5">
-      <c r="A14" s="609"/>
-      <c r="B14" s="609"/>
+      <c r="A14" s="615"/>
+      <c r="B14" s="615"/>
       <c r="C14" s="136" t="s">
         <v>102</v>
       </c>
@@ -18286,8 +18311,8 @@
       <c r="H14" s="84"/>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A15" s="609"/>
-      <c r="B15" s="609"/>
+      <c r="A15" s="615"/>
+      <c r="B15" s="615"/>
       <c r="C15" s="136" t="s">
         <v>689</v>
       </c>
@@ -18300,8 +18325,8 @@
       <c r="H15" s="84"/>
     </row>
     <row r="16" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A16" s="610"/>
-      <c r="B16" s="610"/>
+      <c r="A16" s="616"/>
+      <c r="B16" s="616"/>
       <c r="C16" s="136" t="s">
         <v>104</v>
       </c>
@@ -18449,35 +18474,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>733</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -18492,10 +18517,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -18514,11 +18539,11 @@
         <f>COUNTIF(F$10:F$1007,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1007)</f>
         <v>14</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -18889,35 +18914,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>766</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -18932,10 +18957,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -18954,11 +18979,11 @@
         <f>COUNTIF(F$10:F$1006,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1006)</f>
         <v>13</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -19302,35 +19327,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>780</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -19345,10 +19370,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -19367,11 +19392,11 @@
         <f>COUNTIF(F$10:F$1003,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1003)</f>
         <v>6</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -19430,10 +19455,10 @@
       <c r="H10" s="187"/>
     </row>
     <row r="11" spans="1:8" ht="25.5">
-      <c r="A11" s="608" t="s">
+      <c r="A11" s="614" t="s">
         <v>776</v>
       </c>
-      <c r="B11" s="608" t="s">
+      <c r="B11" s="614" t="s">
         <v>98</v>
       </c>
       <c r="C11" s="135"/>
@@ -19448,8 +19473,8 @@
       <c r="H11" s="187"/>
     </row>
     <row r="12" spans="1:8" ht="25.5">
-      <c r="A12" s="609"/>
-      <c r="B12" s="609"/>
+      <c r="A12" s="615"/>
+      <c r="B12" s="615"/>
       <c r="C12" s="135" t="s">
         <v>775</v>
       </c>
@@ -19462,8 +19487,8 @@
       <c r="H12" s="187"/>
     </row>
     <row r="13" spans="1:8" ht="25.5">
-      <c r="A13" s="609"/>
-      <c r="B13" s="609"/>
+      <c r="A13" s="615"/>
+      <c r="B13" s="615"/>
       <c r="C13" s="135" t="s">
         <v>773</v>
       </c>
@@ -19476,8 +19501,8 @@
       <c r="H13" s="187"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="609"/>
-      <c r="B14" s="609"/>
+      <c r="A14" s="615"/>
+      <c r="B14" s="615"/>
       <c r="C14" s="136" t="s">
         <v>771</v>
       </c>
@@ -19490,8 +19515,8 @@
       <c r="H14" s="187"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="610"/>
-      <c r="B15" s="610"/>
+      <c r="A15" s="616"/>
+      <c r="B15" s="616"/>
       <c r="C15" s="136" t="s">
         <v>104</v>
       </c>
@@ -19638,35 +19663,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>807</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -19681,10 +19706,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -19703,11 +19728,11 @@
         <f>COUNTIF(F$10:F$1005,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1005)</f>
         <v>12</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -20033,35 +20058,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>828</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -20076,10 +20101,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -20098,11 +20123,11 @@
         <f>COUNTIF(F$10:F$1004,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1004)</f>
         <v>11</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -20389,7 +20414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -20406,15 +20431,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="603" t="s">
+      <c r="B1" s="609" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="603"/>
-      <c r="D1" s="603"/>
-      <c r="E1" s="603"/>
-      <c r="F1" s="603"/>
-      <c r="G1" s="603"/>
-      <c r="H1" s="603"/>
+      <c r="C1" s="609"/>
+      <c r="D1" s="609"/>
+      <c r="E1" s="609"/>
+      <c r="F1" s="609"/>
+      <c r="G1" s="609"/>
+      <c r="H1" s="609"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="87"/>
@@ -20430,14 +20455,14 @@
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="600" t="s">
+      <c r="C3" s="606" t="s">
         <v>1316</v>
       </c>
-      <c r="D3" s="600"/>
-      <c r="E3" s="601" t="s">
+      <c r="D3" s="606"/>
+      <c r="E3" s="607" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="601"/>
+      <c r="F3" s="607"/>
       <c r="G3" s="90" t="s">
         <v>1317</v>
       </c>
@@ -20447,14 +20472,14 @@
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="600" t="s">
+      <c r="C4" s="606" t="s">
         <v>1318</v>
       </c>
-      <c r="D4" s="600"/>
-      <c r="E4" s="601" t="s">
+      <c r="D4" s="606"/>
+      <c r="E4" s="607" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="601"/>
+      <c r="F4" s="607"/>
       <c r="G4" s="90"/>
       <c r="H4" s="91"/>
     </row>
@@ -20462,15 +20487,15 @@
       <c r="B5" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="600" t="str">
+      <c r="C5" s="606" t="str">
         <f>C4&amp;"_"&amp;"TestReport"&amp;"_"&amp;"v1.0"</f>
         <v>HTTTNTT_TestReport_v1.0</v>
       </c>
-      <c r="D5" s="600"/>
-      <c r="E5" s="601" t="s">
+      <c r="D5" s="606"/>
+      <c r="E5" s="607" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="601"/>
+      <c r="F5" s="607"/>
       <c r="G5" s="590">
         <v>42562</v>
       </c>
@@ -20481,12 +20506,12 @@
       <c r="B6" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="602"/>
-      <c r="D6" s="602"/>
-      <c r="E6" s="602"/>
-      <c r="F6" s="602"/>
-      <c r="G6" s="602"/>
-      <c r="H6" s="602"/>
+      <c r="C6" s="608"/>
+      <c r="D6" s="608"/>
+      <c r="E6" s="608"/>
+      <c r="F6" s="608"/>
+      <c r="G6" s="608"/>
+      <c r="H6" s="608"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="87"/>
@@ -21598,35 +21623,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>855</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -21641,10 +21666,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -21663,11 +21688,11 @@
         <f>COUNTIF(F$10:F$1001,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1001)</f>
         <v>8</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -21915,35 +21940,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>869</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5" customHeight="1">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -21958,10 +21983,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -21980,11 +22005,11 @@
         <f>COUNTIF(F$10:F$1006,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1006)</f>
         <v>6</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -22043,10 +22068,10 @@
       <c r="H10" s="187"/>
     </row>
     <row r="11" spans="1:8" ht="25.5">
-      <c r="A11" s="608" t="s">
+      <c r="A11" s="614" t="s">
         <v>866</v>
       </c>
-      <c r="B11" s="608" t="s">
+      <c r="B11" s="614" t="s">
         <v>98</v>
       </c>
       <c r="C11" s="135"/>
@@ -22061,8 +22086,8 @@
       <c r="H11" s="187"/>
     </row>
     <row r="12" spans="1:8" ht="25.5">
-      <c r="A12" s="609"/>
-      <c r="B12" s="609"/>
+      <c r="A12" s="615"/>
+      <c r="B12" s="615"/>
       <c r="C12" s="135" t="s">
         <v>865</v>
       </c>
@@ -22075,8 +22100,8 @@
       <c r="H12" s="187"/>
     </row>
     <row r="13" spans="1:8" ht="25.5">
-      <c r="A13" s="609"/>
-      <c r="B13" s="609"/>
+      <c r="A13" s="615"/>
+      <c r="B13" s="615"/>
       <c r="C13" s="135" t="s">
         <v>863</v>
       </c>
@@ -22089,8 +22114,8 @@
       <c r="H13" s="187"/>
     </row>
     <row r="14" spans="1:8" ht="25.5">
-      <c r="A14" s="609"/>
-      <c r="B14" s="609"/>
+      <c r="A14" s="615"/>
+      <c r="B14" s="615"/>
       <c r="C14" s="136" t="s">
         <v>861</v>
       </c>
@@ -22103,8 +22128,8 @@
       <c r="H14" s="187"/>
     </row>
     <row r="15" spans="1:8" ht="25.5">
-      <c r="A15" s="609"/>
-      <c r="B15" s="609"/>
+      <c r="A15" s="615"/>
+      <c r="B15" s="615"/>
       <c r="C15" s="136" t="s">
         <v>100</v>
       </c>
@@ -22117,8 +22142,8 @@
       <c r="H15" s="187"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="619"/>
-      <c r="B16" s="610"/>
+      <c r="A16" s="625"/>
+      <c r="B16" s="616"/>
       <c r="C16" s="136" t="s">
         <v>104</v>
       </c>
@@ -22263,35 +22288,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>899</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -22306,10 +22331,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -22328,11 +22353,11 @@
         <f>COUNTIF(F$10:F$1008,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1008)</f>
         <v>18</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -22769,35 +22794,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>923</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -22812,10 +22837,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -22834,11 +22859,11 @@
         <f>COUNTIF(F$10:F$1008,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1008)</f>
         <v>18</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -23273,35 +23298,35 @@
       <c r="A2" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="622" t="s">
         <v>940</v>
       </c>
-      <c r="C2" s="616"/>
-      <c r="D2" s="616"/>
-      <c r="E2" s="616"/>
-      <c r="F2" s="616"/>
+      <c r="C2" s="622"/>
+      <c r="D2" s="622"/>
+      <c r="E2" s="622"/>
+      <c r="F2" s="622"/>
     </row>
     <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="617" t="s">
+      <c r="B3" s="623" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="617"/>
-      <c r="D3" s="617"/>
-      <c r="E3" s="617"/>
-      <c r="F3" s="617"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="618"/>
-      <c r="C4" s="618"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="624"/>
+      <c r="D4" s="624"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="57" t="s">
@@ -23316,10 +23341,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1">
       <c r="A6" s="83">
@@ -23338,11 +23363,11 @@
         <f>COUNTIF(F$10:F$1007,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1007)</f>
         <v>8</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" s="66" t="s">
@@ -23589,13 +23614,13 @@
       <c r="A2" s="222" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>984</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="249"/>
       <c r="H2" s="246"/>
       <c r="I2" s="247"/>
@@ -23605,13 +23630,13 @@
       <c r="A3" s="223" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="249"/>
       <c r="H3" s="246"/>
       <c r="I3" s="247"/>
@@ -23621,11 +23646,11 @@
       <c r="A4" s="222" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="249"/>
       <c r="H4" s="246"/>
       <c r="I4" s="247"/>
@@ -23644,10 +23669,10 @@
       <c r="D5" s="253" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="620" t="s">
+      <c r="E5" s="626" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="620"/>
+      <c r="F5" s="626"/>
       <c r="G5" s="254"/>
       <c r="H5" s="254"/>
       <c r="I5" s="255"/>
@@ -23666,10 +23691,10 @@
       <c r="D6" s="258">
         <v>0</v>
       </c>
-      <c r="E6" s="621">
+      <c r="E6" s="627">
         <v>4</v>
       </c>
-      <c r="F6" s="621"/>
+      <c r="F6" s="627"/>
       <c r="G6" s="254"/>
       <c r="H6" s="254"/>
       <c r="I6" s="255"/>
@@ -24008,13 +24033,13 @@
       <c r="A2" s="304" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1006</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="335"/>
       <c r="H2" s="332"/>
       <c r="I2" s="333"/>
@@ -24027,13 +24052,13 @@
       <c r="A3" s="305" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="335"/>
       <c r="H3" s="332"/>
       <c r="I3" s="333"/>
@@ -24046,11 +24071,11 @@
       <c r="A4" s="304" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="357"/>
       <c r="H4" s="332"/>
       <c r="I4" s="333"/>
@@ -24072,10 +24097,10 @@
       <c r="D5" s="339" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="620" t="s">
+      <c r="E5" s="626" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="620"/>
+      <c r="F5" s="626"/>
       <c r="G5" s="340"/>
       <c r="H5" s="340"/>
       <c r="I5" s="341"/>
@@ -24097,10 +24122,10 @@
       <c r="D6" s="344">
         <v>0</v>
       </c>
-      <c r="E6" s="621">
+      <c r="E6" s="627">
         <v>3</v>
       </c>
-      <c r="F6" s="621"/>
+      <c r="F6" s="627"/>
       <c r="G6" s="340"/>
       <c r="H6" s="340"/>
       <c r="I6" s="341"/>
@@ -24458,13 +24483,13 @@
       <c r="A2" s="375" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1024</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="399"/>
       <c r="H2" s="396"/>
       <c r="I2" s="397"/>
@@ -24474,13 +24499,13 @@
       <c r="A3" s="376" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="399"/>
       <c r="H3" s="396"/>
       <c r="I3" s="397"/>
@@ -24490,11 +24515,11 @@
       <c r="A4" s="375" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="399"/>
       <c r="H4" s="396"/>
       <c r="I4" s="397"/>
@@ -24513,10 +24538,10 @@
       <c r="D5" s="403" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="620" t="s">
+      <c r="E5" s="626" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="620"/>
+      <c r="F5" s="626"/>
       <c r="G5" s="404"/>
       <c r="H5" s="404"/>
       <c r="I5" s="405"/>
@@ -24535,10 +24560,10 @@
       <c r="D6" s="407">
         <v>0</v>
       </c>
-      <c r="E6" s="621">
+      <c r="E6" s="627">
         <v>15</v>
       </c>
-      <c r="F6" s="621"/>
+      <c r="F6" s="627"/>
       <c r="G6" s="404"/>
       <c r="H6" s="404"/>
       <c r="I6" s="405"/>
@@ -24975,13 +25000,13 @@
       <c r="A2" s="433" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1075</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="467"/>
       <c r="H2" s="464"/>
       <c r="I2" s="465"/>
@@ -24992,13 +25017,13 @@
       <c r="A3" s="434" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="467"/>
       <c r="H3" s="464"/>
       <c r="I3" s="465"/>
@@ -25009,11 +25034,11 @@
       <c r="A4" s="433" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="467"/>
       <c r="H4" s="464"/>
       <c r="I4" s="465"/>
@@ -25033,10 +25058,10 @@
       <c r="D5" s="471" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="620" t="s">
+      <c r="E5" s="626" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="620"/>
+      <c r="F5" s="626"/>
       <c r="G5" s="472"/>
       <c r="H5" s="472"/>
       <c r="I5" s="473"/>
@@ -25056,10 +25081,10 @@
       <c r="D6" s="476">
         <v>0</v>
       </c>
-      <c r="E6" s="621">
+      <c r="E6" s="627">
         <v>3</v>
       </c>
-      <c r="F6" s="621"/>
+      <c r="F6" s="627"/>
       <c r="G6" s="472"/>
       <c r="H6" s="472"/>
       <c r="I6" s="473"/>
@@ -25391,13 +25416,13 @@
       <c r="A2" s="507" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>1300</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="534"/>
       <c r="H2" s="531"/>
       <c r="I2" s="532"/>
@@ -25407,13 +25432,13 @@
       <c r="A3" s="508" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="534"/>
       <c r="H3" s="531"/>
       <c r="I3" s="532"/>
@@ -25423,11 +25448,11 @@
       <c r="A4" s="507" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="534"/>
       <c r="H4" s="531"/>
       <c r="I4" s="532"/>
@@ -25446,10 +25471,10 @@
       <c r="D5" s="537" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="620" t="s">
+      <c r="E5" s="626" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="620"/>
+      <c r="F5" s="626"/>
       <c r="G5" s="538"/>
       <c r="H5" s="538"/>
       <c r="I5" s="539"/>
@@ -25468,10 +25493,10 @@
       <c r="D6" s="541">
         <v>0</v>
       </c>
-      <c r="E6" s="621">
+      <c r="E6" s="627">
         <v>5</v>
       </c>
-      <c r="F6" s="621"/>
+      <c r="F6" s="627"/>
       <c r="G6" s="538"/>
       <c r="H6" s="538"/>
       <c r="I6" s="539"/>
@@ -25799,13 +25824,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -25817,13 +25842,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -25835,11 +25860,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -25858,10 +25883,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -25886,11 +25911,11 @@
         <f>COUNTIF(F$10:F$1002,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1002)</f>
         <v>11</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -26259,13 +26284,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -26277,13 +26302,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -26295,11 +26320,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -26318,10 +26343,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -26346,11 +26371,11 @@
         <f>COUNTIF(F$10:F$1005,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1005)</f>
         <v>13</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -26426,10 +26451,10 @@
       <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="608" t="s">
+      <c r="A11" s="614" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="608" t="s">
+      <c r="B11" s="614" t="s">
         <v>98</v>
       </c>
       <c r="C11" s="135"/>
@@ -26445,8 +26470,8 @@
       <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="609"/>
-      <c r="B12" s="609"/>
+      <c r="A12" s="615"/>
+      <c r="B12" s="615"/>
       <c r="C12" s="135" t="s">
         <v>100</v>
       </c>
@@ -26460,8 +26485,8 @@
       <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="609"/>
-      <c r="B13" s="609"/>
+      <c r="A13" s="615"/>
+      <c r="B13" s="615"/>
       <c r="C13" s="135" t="s">
         <v>101</v>
       </c>
@@ -26475,8 +26500,8 @@
       <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="609"/>
-      <c r="B14" s="609"/>
+      <c r="A14" s="615"/>
+      <c r="B14" s="615"/>
       <c r="C14" s="136" t="s">
         <v>102</v>
       </c>
@@ -26490,8 +26515,8 @@
       <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:10" ht="25.5">
-      <c r="A15" s="609"/>
-      <c r="B15" s="609"/>
+      <c r="A15" s="615"/>
+      <c r="B15" s="615"/>
       <c r="C15" s="136" t="s">
         <v>103</v>
       </c>
@@ -26505,8 +26530,8 @@
       <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="610"/>
-      <c r="B16" s="610"/>
+      <c r="A16" s="616"/>
+      <c r="B16" s="616"/>
       <c r="C16" s="136" t="s">
         <v>104</v>
       </c>
@@ -26632,8 +26657,8 @@
       <c r="I22" s="82"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="622"/>
-      <c r="B23" s="622" t="s">
+      <c r="A23" s="593"/>
+      <c r="B23" s="593" t="s">
         <v>135</v>
       </c>
       <c r="C23" s="370"/>
@@ -26641,7 +26666,7 @@
       <c r="E23" s="370"/>
       <c r="F23" s="370"/>
       <c r="G23" s="370"/>
-      <c r="H23" s="623"/>
+      <c r="H23" s="594"/>
       <c r="I23" s="72"/>
       <c r="J23" s="52"/>
       <c r="K23" s="52"/>
@@ -26650,13 +26675,13 @@
       <c r="A24" s="169" t="s">
         <v>1321</v>
       </c>
-      <c r="B24" s="624" t="s">
+      <c r="B24" s="595" t="s">
         <v>1322</v>
       </c>
-      <c r="C24" s="625" t="s">
+      <c r="C24" s="596" t="s">
         <v>1323</v>
       </c>
-      <c r="D24" s="626" t="s">
+      <c r="D24" s="597" t="s">
         <v>1324</v>
       </c>
       <c r="E24" s="169"/>
@@ -26668,8 +26693,8 @@
       <c r="I24" s="77"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="622"/>
-      <c r="B25" s="622" t="s">
+      <c r="A25" s="593"/>
+      <c r="B25" s="593" t="s">
         <v>759</v>
       </c>
       <c r="C25" s="370"/>
@@ -26677,19 +26702,19 @@
       <c r="E25" s="370"/>
       <c r="F25" s="370"/>
       <c r="G25" s="370"/>
-      <c r="H25" s="623"/>
+      <c r="H25" s="594"/>
     </row>
     <row r="26" spans="1:11" ht="38.25">
       <c r="A26" s="169" t="s">
         <v>1325</v>
       </c>
-      <c r="B26" s="624" t="s">
+      <c r="B26" s="595" t="s">
         <v>1326</v>
       </c>
-      <c r="C26" s="625" t="s">
+      <c r="C26" s="596" t="s">
         <v>1327</v>
       </c>
-      <c r="D26" s="626" t="s">
+      <c r="D26" s="597" t="s">
         <v>1328</v>
       </c>
       <c r="E26" s="169"/>
@@ -26700,8 +26725,8 @@
       <c r="H26" s="169"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="622"/>
-      <c r="B27" s="622" t="s">
+      <c r="A27" s="593"/>
+      <c r="B27" s="593" t="s">
         <v>1329</v>
       </c>
       <c r="C27" s="370"/>
@@ -26709,19 +26734,19 @@
       <c r="E27" s="370"/>
       <c r="F27" s="370"/>
       <c r="G27" s="370"/>
-      <c r="H27" s="623"/>
+      <c r="H27" s="594"/>
     </row>
     <row r="28" spans="1:11" ht="38.25">
       <c r="A28" s="169" t="s">
         <v>1330</v>
       </c>
-      <c r="B28" s="624" t="s">
+      <c r="B28" s="595" t="s">
         <v>1331</v>
       </c>
-      <c r="C28" s="625" t="s">
+      <c r="C28" s="596" t="s">
         <v>1332</v>
       </c>
-      <c r="D28" s="625" t="s">
+      <c r="D28" s="596" t="s">
         <v>1333</v>
       </c>
       <c r="E28" s="169"/>
@@ -26731,17 +26756,17 @@
       <c r="G28" s="171"/>
       <c r="H28" s="169"/>
     </row>
-    <row r="29" spans="1:11" ht="51">
+    <row r="29" spans="1:11" ht="38.25">
       <c r="A29" s="169" t="s">
         <v>1334</v>
       </c>
-      <c r="B29" s="624" t="s">
+      <c r="B29" s="595" t="s">
         <v>1335</v>
       </c>
-      <c r="C29" s="625" t="s">
+      <c r="C29" s="596" t="s">
         <v>1332</v>
       </c>
-      <c r="D29" s="625" t="s">
+      <c r="D29" s="596" t="s">
         <v>1336</v>
       </c>
       <c r="E29" s="169"/>
@@ -26752,8 +26777,8 @@
       <c r="H29" s="169"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="622"/>
-      <c r="B30" s="622" t="s">
+      <c r="A30" s="593"/>
+      <c r="B30" s="593" t="s">
         <v>1339</v>
       </c>
       <c r="C30" s="370"/>
@@ -26761,19 +26786,19 @@
       <c r="E30" s="370"/>
       <c r="F30" s="370"/>
       <c r="G30" s="370"/>
-      <c r="H30" s="623"/>
+      <c r="H30" s="594"/>
     </row>
     <row r="31" spans="1:11" ht="51">
       <c r="A31" s="169" t="s">
         <v>1340</v>
       </c>
-      <c r="B31" s="624" t="s">
+      <c r="B31" s="595" t="s">
         <v>1341</v>
       </c>
-      <c r="C31" s="625" t="s">
+      <c r="C31" s="596" t="s">
         <v>1342</v>
       </c>
-      <c r="D31" s="626" t="s">
+      <c r="D31" s="597" t="s">
         <v>1343</v>
       </c>
       <c r="E31" s="169"/>
@@ -26787,13 +26812,13 @@
       <c r="A32" s="169" t="s">
         <v>1344</v>
       </c>
-      <c r="B32" s="624" t="s">
+      <c r="B32" s="595" t="s">
         <v>1345</v>
       </c>
-      <c r="C32" s="625" t="s">
+      <c r="C32" s="596" t="s">
         <v>1346</v>
       </c>
-      <c r="D32" s="625" t="s">
+      <c r="D32" s="596" t="s">
         <v>1347</v>
       </c>
       <c r="E32" s="169"/>
@@ -26868,13 +26893,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -26886,13 +26911,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -26904,11 +26929,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -26927,10 +26952,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -26955,11 +26980,11 @@
         <f>COUNTIF(F$10:F$1008,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1009)</f>
         <v>16</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -27165,7 +27190,7 @@
       <c r="H17" s="81"/>
       <c r="I17" s="77"/>
     </row>
-    <row r="18" spans="1:11" ht="76.5">
+    <row r="18" spans="1:11" ht="63.75">
       <c r="A18" s="73" t="s">
         <v>187</v>
       </c>
@@ -27186,7 +27211,7 @@
       <c r="H18" s="81"/>
       <c r="I18" s="77"/>
     </row>
-    <row r="19" spans="1:11" ht="76.5">
+    <row r="19" spans="1:11" ht="63.75">
       <c r="A19" s="73" t="s">
         <v>188</v>
       </c>
@@ -27270,7 +27295,7 @@
       <c r="H22" s="81"/>
       <c r="I22" s="77"/>
     </row>
-    <row r="23" spans="1:11" ht="76.5">
+    <row r="23" spans="1:11" ht="63.75">
       <c r="A23" s="73" t="s">
         <v>192</v>
       </c>
@@ -27429,13 +27454,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -27447,13 +27472,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -27465,11 +27490,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -27488,10 +27513,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -27516,11 +27541,11 @@
         <f>COUNTIF(F$10:F$1011,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <f>COUNTA(A10:A1012)</f>
         <v>19</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -27892,7 +27917,7 @@
       <c r="H25" s="81"/>
       <c r="I25" s="77"/>
     </row>
-    <row r="26" spans="1:11" ht="76.5">
+    <row r="26" spans="1:11" ht="63.75">
       <c r="A26" s="73" t="s">
         <v>873</v>
       </c>
@@ -28042,13 +28067,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -28060,13 +28085,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -28078,11 +28103,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -28101,10 +28126,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -28128,10 +28153,10 @@
         <f>COUNTIF(F$10:F$1004,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>6</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>
@@ -28207,10 +28232,10 @@
       <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="608" t="s">
+      <c r="A11" s="614" t="s">
         <v>230</v>
       </c>
-      <c r="B11" s="608" t="s">
+      <c r="B11" s="614" t="s">
         <v>98</v>
       </c>
       <c r="C11" s="135"/>
@@ -28226,8 +28251,8 @@
       <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="609"/>
-      <c r="B12" s="609"/>
+      <c r="A12" s="615"/>
+      <c r="B12" s="615"/>
       <c r="C12" s="135" t="s">
         <v>222</v>
       </c>
@@ -28241,8 +28266,8 @@
       <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="609"/>
-      <c r="B13" s="609"/>
+      <c r="A13" s="615"/>
+      <c r="B13" s="615"/>
       <c r="C13" s="135" t="s">
         <v>223</v>
       </c>
@@ -28256,8 +28281,8 @@
       <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="609"/>
-      <c r="B14" s="609"/>
+      <c r="A14" s="615"/>
+      <c r="B14" s="615"/>
       <c r="C14" s="136" t="s">
         <v>224</v>
       </c>
@@ -28271,8 +28296,8 @@
       <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:10" ht="25.5">
-      <c r="A15" s="609"/>
-      <c r="B15" s="609"/>
+      <c r="A15" s="615"/>
+      <c r="B15" s="615"/>
       <c r="C15" s="136" t="s">
         <v>225</v>
       </c>
@@ -28286,8 +28311,8 @@
       <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="610"/>
-      <c r="B16" s="610"/>
+      <c r="A16" s="616"/>
+      <c r="B16" s="616"/>
       <c r="C16" s="136" t="s">
         <v>104</v>
       </c>
@@ -28462,13 +28487,13 @@
       <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="605" t="s">
+      <c r="B2" s="611" t="s">
         <v>236</v>
       </c>
-      <c r="C2" s="605"/>
-      <c r="D2" s="605"/>
-      <c r="E2" s="605"/>
-      <c r="F2" s="605"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
+      <c r="E2" s="611"/>
+      <c r="F2" s="611"/>
       <c r="G2" s="54"/>
       <c r="H2" s="40"/>
       <c r="I2" s="51"/>
@@ -28480,13 +28505,13 @@
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="605" t="s">
+      <c r="B3" s="611" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="605"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="605"/>
-      <c r="F3" s="605"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
+      <c r="E3" s="611"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="54"/>
       <c r="H3" s="40"/>
       <c r="I3" s="51"/>
@@ -28498,11 +28523,11 @@
       <c r="A4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="606"/>
-      <c r="C4" s="606"/>
-      <c r="D4" s="606"/>
-      <c r="E4" s="606"/>
-      <c r="F4" s="606"/>
+      <c r="B4" s="612"/>
+      <c r="C4" s="612"/>
+      <c r="D4" s="612"/>
+      <c r="E4" s="612"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="54"/>
       <c r="H4" s="40"/>
       <c r="I4" s="51"/>
@@ -28521,10 +28546,10 @@
       <c r="D5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="607" t="s">
+      <c r="E5" s="613" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="607"/>
+      <c r="F5" s="613"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="61"/>
@@ -28548,10 +28573,10 @@
         <f>COUNTIF(F$10:F$1010,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="604">
+      <c r="E6" s="610">
         <v>16</v>
       </c>
-      <c r="F6" s="604"/>
+      <c r="F6" s="610"/>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
       <c r="I6" s="61"/>

</xml_diff>